<commit_message>
clustering and association update
</commit_message>
<xml_diff>
--- a/Project3/clustering_errors.xlsx
+++ b/Project3/clustering_errors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>AIC</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>CVE</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -380,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,285 +399,25 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>35718.8071671121</v>
+        <v>10750725.75768713</v>
       </c>
       <c r="C2">
-        <v>36553.12556453906</v>
+        <v>10764514.47884863</v>
       </c>
       <c r="D2">
-        <v>18173.08410391211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>-37572.35111791521</v>
-      </c>
-      <c r="C3">
-        <v>-35898.8065677823</v>
-      </c>
-      <c r="D3">
-        <v>498037.4120100702</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>-2922.701031787561</v>
-      </c>
-      <c r="C4">
-        <v>-409.930328948707</v>
-      </c>
-      <c r="D4">
-        <v>1997083.14063157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>-15381.62288926496</v>
-      </c>
-      <c r="C5">
-        <v>-12029.62603372016</v>
-      </c>
-      <c r="D5">
-        <v>3988749.872027857</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>-27694.22199312333</v>
-      </c>
-      <c r="C6">
-        <v>-23502.99898487259</v>
-      </c>
-      <c r="D6">
-        <v>3487062.016652425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>-35206.34934204662</v>
-      </c>
-      <c r="C7">
-        <v>-30175.90018108993</v>
-      </c>
-      <c r="D7">
-        <v>2481246.983729417</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>-59680.5317612769</v>
-      </c>
-      <c r="C8">
-        <v>-53810.85644761426</v>
-      </c>
-      <c r="D8">
-        <v>11477182.84925053</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>-73129.04736677284</v>
-      </c>
-      <c r="C9">
-        <v>-66420.14590040426</v>
-      </c>
-      <c r="D9">
-        <v>21463118.83930168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>-81638.78319186677</v>
-      </c>
-      <c r="C10">
-        <v>-74090.65557279224</v>
-      </c>
-      <c r="D10">
-        <v>27457255.00299338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>-89491.28181977112</v>
-      </c>
-      <c r="C11">
-        <v>-81103.92804799064</v>
-      </c>
-      <c r="D11">
-        <v>30446163.02187569</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>-115255.3884553321</v>
-      </c>
-      <c r="C12">
-        <v>-106028.8085308457</v>
-      </c>
-      <c r="D12">
-        <v>44442950.91875927</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>-122348.1144978759</v>
-      </c>
-      <c r="C13">
-        <v>-112282.3084206836</v>
-      </c>
-      <c r="D13">
-        <v>53935909.65228787</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>-159150.1332915042</v>
-      </c>
-      <c r="C14">
-        <v>-148245.1010616059</v>
-      </c>
-      <c r="D14">
-        <v>57930455.20910468</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>-147782.9476598708</v>
-      </c>
-      <c r="C15">
-        <v>-136038.6892772665</v>
-      </c>
-      <c r="D15">
-        <v>84920646.03697875</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>-147370.666490901</v>
-      </c>
-      <c r="C16">
-        <v>-134787.1819555908</v>
-      </c>
-      <c r="D16">
-        <v>82417762.84685767</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>-171861.9037733979</v>
-      </c>
-      <c r="C17">
-        <v>-158439.1930853818</v>
-      </c>
-      <c r="D17">
-        <v>82412635.88789865</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>-181740.1207644173</v>
-      </c>
-      <c r="C18">
-        <v>-167478.1839236952</v>
-      </c>
-      <c r="D18">
-        <v>82411825.00481224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>-185568.8498622605</v>
-      </c>
-      <c r="C19">
-        <v>-170467.6868688325</v>
-      </c>
-      <c r="D19">
-        <v>91409668.71808305</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>-205243.4718679893</v>
-      </c>
-      <c r="C20">
-        <v>-189303.0827218553</v>
-      </c>
-      <c r="D20">
-        <v>88407846.02617949</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>-194097.0945944391</v>
-      </c>
-      <c r="C21">
-        <v>-177317.4792955991</v>
-      </c>
-      <c r="D21">
-        <v>92402718.15856965</v>
+        <v>10744753.67517034</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>